<commit_message>
STUDY - 4 ThreadLocal学习
</commit_message>
<xml_diff>
--- a/doc/学习记录.xlsx
+++ b/doc/学习记录.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeOfCompany\IDEA\MayDay\Project\study\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F42AB1-A59F-47CE-B344-2CA27B78D2ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7E1077-6398-414B-9C89-BF6AF479777C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RabbitMQ" sheetId="1" r:id="rId1"/>
+    <sheet name="ThreadLocal" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>学习简介</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,6 +61,30 @@
   </si>
   <si>
     <t>最新安装包rabbit.exe 下载了多次，难下载</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习ThreadLocal,使用Apache2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花费6个小时左右</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>windows 中安装Apache2，并使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花费6小时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周五</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习ThreadLocal源码，子编写ThreadLocal</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -388,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -456,4 +481,70 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B9D5F9-C915-4C26-9875-7D55E5B4FDBA}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>44043</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>44045</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
STUDY - 2 effectivite 学习记录add
</commit_message>
<xml_diff>
--- a/doc/学习记录.xlsx
+++ b/doc/学习记录.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeOfCompany\IDEA\MayDay\Project\study\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7E1077-6398-414B-9C89-BF6AF479777C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72777440-3106-419F-819E-FEF42F7F2926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7470" yWindow="1980" windowWidth="22110" windowHeight="13200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RabbitMQ" sheetId="1" r:id="rId1"/>
     <sheet name="ThreadLocal" sheetId="2" r:id="rId2"/>
+    <sheet name="quartz" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>学习简介</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,7 +85,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>学习ThreadLocal源码，子编写ThreadLocal</t>
+    <t>博客学习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花费3小时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周四</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>源码查看</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花费5小时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载源码，查看使用方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习ThreadLocal源码，自编写ThreadLocal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quartz 模型搭建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官方文档</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运行bug fix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>排查问题并验证</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -137,6 +182,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -156,7 +269,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -414,7 +527,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -485,10 +598,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B9D5F9-C915-4C26-9875-7D55E5B4FDBA}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -533,7 +646,7 @@
         <v>44045</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -541,10 +654,112 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DAAA8E-B631-428F-976B-546AEADB427E}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>44101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>44102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>44112</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>44115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>44117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>